<commit_message>
Add two function importCoursesSchedulesOfAClass(19) and addACourseSchedule(20)
</commit_message>
<xml_diff>
--- a/CS Project/Courses-Schedule.xlsx
+++ b/CS Project/Courses-Schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studenthcmusedu-my.sharepoint.com/personal/1751027_student_hcmus_edu_vn/Documents/APCS/Computer Science/Project Final/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huung\OneDrive\Documents\GitHub\CS-Project\CS Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E9EFFE8-5AE4-43BA-B297-2A61D42DD57A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="6_{368D03C3-6FB2-44CC-9A64-3747F5B2204B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{315D2FD4-4686-42BF-8FC5-4FC8F55EA3EA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Course code</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>Nguyễn Hữu Anh</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>I42</t>
   </si>
 </sst>
 </file>
@@ -435,25 +441,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D9C755-FC61-495A-98EE-D76D5E55559B}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7265625" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" customWidth="1"/>
-    <col min="3" max="3" width="21.1796875" customWidth="1"/>
-    <col min="4" max="4" width="7.08984375" customWidth="1"/>
-    <col min="6" max="6" width="10.90625" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.36328125" customWidth="1"/>
-    <col min="9" max="9" width="9.26953125" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" customWidth="1"/>
+    <col min="3" max="3" width="21.21875" customWidth="1"/>
+    <col min="4" max="4" width="7.109375" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
+    <col min="9" max="9" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -484,8 +490,11 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -516,8 +525,11 @@
       <c r="J2" s="2">
         <v>0.375</v>
       </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -548,8 +560,11 @@
       <c r="J3" s="2">
         <v>0.47916666666666669</v>
       </c>
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -579,6 +594,9 @@
       </c>
       <c r="J4" s="2">
         <v>0.375</v>
+      </c>
+      <c r="K4" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>